<commit_message>
added schematics, updated part estimate
</commit_message>
<xml_diff>
--- a/part count estimates.xlsx
+++ b/part count estimates.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7D03DD-8071-4A13-8A3F-9F1431B78CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055D2DD0-B5D7-41D1-8C85-70CE2292C790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="31">
   <si>
     <t>Register File</t>
   </si>
@@ -51,13 +52,73 @@
     <t>-</t>
   </si>
   <si>
-    <t>LED red</t>
-  </si>
-  <si>
     <t>Program Counter</t>
   </si>
   <si>
     <t>Adder</t>
+  </si>
+  <si>
+    <t>Hold unit</t>
+  </si>
+  <si>
+    <t>LED r 5mm</t>
+  </si>
+  <si>
+    <t>LED g 3mm</t>
+  </si>
+  <si>
+    <t>LED r 3mm</t>
+  </si>
+  <si>
+    <t>2k 0805</t>
+  </si>
+  <si>
+    <t>Condition unit</t>
+  </si>
+  <si>
+    <t>1bit</t>
+  </si>
+  <si>
+    <t>XOR 4x2in</t>
+  </si>
+  <si>
+    <t>AND 1x2in</t>
+  </si>
+  <si>
+    <t>NOT 4x1in</t>
+  </si>
+  <si>
+    <t>OR 4x2in</t>
+  </si>
+  <si>
+    <t>Load unit</t>
+  </si>
+  <si>
+    <t>IO unit</t>
+  </si>
+  <si>
+    <t>Arithmetic unit</t>
+  </si>
+  <si>
+    <t>MUX 8-&gt;1</t>
+  </si>
+  <si>
+    <t>Shift unit</t>
+  </si>
+  <si>
+    <t>Logic unit</t>
+  </si>
+  <si>
+    <t>xdxdxd</t>
+  </si>
+  <si>
+    <t>4x2 AND, OR, XOR, NAND, NOR, XNOR 2 each</t>
+  </si>
+  <si>
+    <t>Steckbretter</t>
+  </si>
+  <si>
+    <t>30?</t>
   </si>
 </sst>
 </file>
@@ -93,8 +154,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -375,20 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.86328125" customWidth="1"/>
     <col min="2" max="4" width="10.1328125" customWidth="1"/>
-    <col min="6" max="9" width="10.1328125" customWidth="1"/>
+    <col min="7" max="8" width="10.1328125" customWidth="1"/>
+    <col min="14" max="15" width="10.1328125" customWidth="1"/>
+    <col min="16" max="16" width="48.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -399,97 +466,549 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>24</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="L3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="1">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1">
+        <v>8</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D4D446-9A88-47A6-A1CD-687F42807662}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.53125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added parts for breadboard version
</commit_message>
<xml_diff>
--- a/part count estimates.xlsx
+++ b/part count estimates.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\computer\ax08-pc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2387492-DDA0-4988-954E-CABB2EE6E12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F668EE-EB59-4F21-A2F4-509AA7F4DD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="part_links" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="part_links" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
   <si>
     <t>Register File</t>
   </si>
@@ -83,9 +82,6 @@
     <t>LED r 3mm</t>
   </si>
   <si>
-    <t>2k 0805</t>
-  </si>
-  <si>
     <t>Condition unit</t>
   </si>
   <si>
@@ -128,12 +124,6 @@
     <t>4x2 AND, OR, XOR, NAND, NOR, XNOR 2 each</t>
   </si>
   <si>
-    <t>Steckbretter</t>
-  </si>
-  <si>
-    <t>30?</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -165,6 +155,216 @@
   </si>
   <si>
     <t>Nur Peter</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>SN74HC245N</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Buffers-Drivers-Receivers-Transceivers_Texas-Instruments-SN74HC245N_C2899.html</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Latches_lingxingic-SN74LS373N-LX_C22374106.html</t>
+  </si>
+  <si>
+    <t>SN74LS373N(LX)</t>
+  </si>
+  <si>
+    <t>SN74LS283N(LX)</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Specialty-Logic_lingxingic-SN74LS283N-LX_C22374104.html</t>
+  </si>
+  <si>
+    <t>SN74HC157N(LX)</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Signal-Switches-Multiplexers-Decoders_lingxingic-SN74HC157N-LX_C22436657.html</t>
+  </si>
+  <si>
+    <t>SN74LS32N(LX)</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Logic-Gates_lingxingic-SN74LS32N-LX_C22466295.html</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Logic-Gates_lingxingic-SN74LS86AN-LX_C22466310.html</t>
+  </si>
+  <si>
+    <t>SN74LS86AN(LX)</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Logic-Gates_lingxingic-SN74LS08N-LX_C22384768.html</t>
+  </si>
+  <si>
+    <t>SN74LS08N(LX)</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Logic-Gates_lingxingic-SN74LS00N-LX_C22374089.html</t>
+  </si>
+  <si>
+    <t>SN74LS00N(LX)</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Logic-Gates_lingxingic-SN74LS02N-LX_C22374091.html</t>
+  </si>
+  <si>
+    <t>SN74LS02N(LX)</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Logic-Gates_lingxingic-CD4077BE-LX_C24833629.html</t>
+  </si>
+  <si>
+    <t>CD4077BE(LX)</t>
+  </si>
+  <si>
+    <t>XNOR</t>
+  </si>
+  <si>
+    <t>NOR</t>
+  </si>
+  <si>
+    <t>NAND</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t>multiplexer</t>
+  </si>
+  <si>
+    <t>full adder</t>
+  </si>
+  <si>
+    <t>D latch</t>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>DS1136-06-830SNV</t>
+  </si>
+  <si>
+    <t>breadboard</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/PCBs-Breadboards_CONNFLY-Elec-DS1136-06-830SNV_C93726.html</t>
+  </si>
+  <si>
+    <t>DY-333SDRD-SN-A3(EL)(HF)</t>
+  </si>
+  <si>
+    <t>LED red 5mm</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/LED-Indication-Discrete_TONYU-DY-333SDRD-SN-A3-EL-HF_C7470717.html</t>
+  </si>
+  <si>
+    <t>DY-204UYGD-H38-A3</t>
+  </si>
+  <si>
+    <t>LED green 3mm</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/LED-Indication-Discrete_TONYU-DY-204UYGD-H38-A3_C7470727.html</t>
+  </si>
+  <si>
+    <t>LED red 3mm</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/LED-Indication-Discrete_Lite-On-LTL17KRH5D-012A_C7435538.html</t>
+  </si>
+  <si>
+    <t>LTL17KRH5D-012A</t>
+  </si>
+  <si>
+    <t>PM254-1-10-Z-8.5</t>
+  </si>
+  <si>
+    <t>pin header 10 f</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Female-Headers_HCTL-PM254-1-10-Z-8-5_C2897373.html</t>
+  </si>
+  <si>
+    <t>XFCN PZ254R-11-10P</t>
+  </si>
+  <si>
+    <t>pin header 10 m 90°</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Pin-Headers_XFCN-PZ254R-11-10P_C492418.html</t>
+  </si>
+  <si>
+    <t>buffer for debugger</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Buffers-Drivers-Receivers-Transceivers_XBLW-SN74LS244N-XBLW_C42451381.html</t>
+  </si>
+  <si>
+    <t>SN74LS244N(XBLW)</t>
+  </si>
+  <si>
+    <t>RC0805FR-072KL</t>
+  </si>
+  <si>
+    <t>resistor 2k 0805</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_YAGEO-RC0805FR-072KL_C114572.html</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_YAGEO-CC0805KRX7R9BB104_C49678.html</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>capacitor 100nF 0805</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Samsung-Electro-Mechanics-CL21B334KBFNNNE_C73142.html</t>
+  </si>
+  <si>
+    <t>CL21B334KBFNNNE</t>
+  </si>
+  <si>
+    <t>capacitor 330nF 0805</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/IDC-Connectors_BOOMELE-Boom-Precision-Elec-2-54-2-4P_C9135.html</t>
+  </si>
+  <si>
+    <t>IDC connector</t>
+  </si>
+  <si>
+    <t>2.54-2*4P</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Dupont-wire-terminal-block-wire-electronic-wire_DEALON-IDC-265126-200-8P_C7465809.html</t>
+  </si>
+  <si>
+    <t>IDC cable</t>
+  </si>
+  <si>
+    <t>IDC-265126-200-8P</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Inverters_lingxingic-SN74LS04N-LX_C22374093.html</t>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>SN74LS04N(LX)</t>
   </si>
 </sst>
 </file>
@@ -249,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -262,10 +462,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -543,22 +744,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="4" width="10.140625" customWidth="1"/>
-    <col min="7" max="8" width="10.140625" customWidth="1"/>
-    <col min="14" max="15" width="10.140625" customWidth="1"/>
-    <col min="16" max="16" width="48.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="4" width="10.1328125" customWidth="1"/>
+    <col min="7" max="8" width="10.1328125" customWidth="1"/>
+    <col min="14" max="15" width="10.1328125" customWidth="1"/>
+    <col min="16" max="16" width="48.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -572,19 +771,19 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>
@@ -602,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -652,7 +851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -699,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -746,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -793,15 +992,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -840,9 +1039,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -887,9 +1086,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -934,9 +1133,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -981,9 +1180,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -1028,9 +1227,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1">
         <v>6</v>
@@ -1075,7 +1274,68 @@
         <v>7</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B2:B11)</f>
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:O13" si="0">SUM(C2:C11)</f>
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1084,94 +1344,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D4D446-9A88-47A6-A1CD-687F42807662}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2F25C3-A040-4D55-A5F0-DFC308DB6F13}">
+  <dimension ref="B1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1"/>
+    <col min="2" max="2" width="26.86328125" customWidth="1"/>
+    <col min="3" max="3" width="29.73046875" customWidth="1"/>
+    <col min="6" max="6" width="109.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2F25C3-A040-4D55-A5F0-DFC308DB6F13}">
-  <dimension ref="B1:K6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="109.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
         <v>38</v>
-      </c>
-      <c r="J1" t="s">
-        <v>41</v>
       </c>
       <c r="K1" s="4">
         <f>2*E5</f>
         <v>10.8</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="H2" s="4">
-        <f>SUM(H5:H995)</f>
-        <v>62.199999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>SUM(H5:H996)</f>
+        <v>144.58160000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="4" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" t="str">
         <f>"+2 für Peter"</f>
@@ -1184,16 +1409,16 @@
         <v>5.4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" s="4">
         <f>D5*E5</f>
         <v>21.6</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -1201,39 +1426,547 @@
       <c r="E6" s="4">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F6" t="s">
-        <v>39</v>
+      <c r="F6" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="H6" s="4">
         <f>D6*E6</f>
         <v>40.599999999999994</v>
       </c>
     </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.31519999999999998</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="4">
+        <f>D7*E7</f>
+        <v>17.335999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.38229999999999997</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="4">
+        <f>D8*E8</f>
+        <v>7.645999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.27639999999999998</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="8">
+        <f>D9*E9</f>
+        <v>2.7639999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.24179999999999999</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="8">
+        <f>D10*E10</f>
+        <v>1.2089999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.15010000000000001</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="8">
+        <f>D11*E11</f>
+        <v>0.75050000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.18709999999999999</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="8">
+        <f>D12*E12</f>
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.1709</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="8">
+        <f>D13*E13</f>
+        <v>0.85450000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.15359999999999999</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="8">
+        <f>D14*E14</f>
+        <v>0.7679999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.2198</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="8">
+        <f>D15*E15</f>
+        <v>1.099</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.17979999999999999</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="8">
+        <f>D16*E16</f>
+        <v>0.89899999999999991</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.2011</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="8">
+        <f>D17*E17</f>
+        <v>2.0110000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.3764000000000001</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="8">
+        <f>D18*E18</f>
+        <v>27.528000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="8">
+        <f>D19*E19</f>
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20">
+        <v>200</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="8">
+        <f>D20*E20</f>
+        <v>4.7600000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21">
+        <v>100</v>
+      </c>
+      <c r="E21" s="4">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="8">
+        <f>D21*E21</f>
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.13320000000000001</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="8">
+        <f>D22*E22</f>
+        <v>1.3320000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4">
+        <v>4.58E-2</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="8">
+        <f>D23*E23</f>
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.2238</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="8">
+        <f>D24*E24</f>
+        <v>2.6856</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25">
+        <v>200</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1.8E-3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="8">
+        <f>D25*E25</f>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26">
+        <v>300</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" s="8">
+        <f>D26*E26</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="8">
+        <f>D27*E27</f>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>7.2099999999999997E-2</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="8">
+        <f>D28*E28</f>
+        <v>0.36049999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.2525</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="8">
+        <f>D29*E29</f>
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H33" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{9B4F13C2-FDF0-49B6-A1DF-4BA6103DA2A4}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{9450BCB2-A296-4CA3-BAA0-4AC462464BA8}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{F41B1284-5885-45C9-BE63-85B360F38F23}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{69FEB51F-05C6-4D91-8BA5-CA2EB925D7C3}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{54DFEC09-A616-4728-A128-48AD78049813}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{2671F9C5-BD86-410A-8F6F-8799ECDB9148}"/>
+    <hyperlink ref="F11" r:id="rId7" xr:uid="{57A3C39E-B338-4133-A91E-C941732AC0B0}"/>
+    <hyperlink ref="F12" r:id="rId8" xr:uid="{55FD41B5-5832-4288-A7E6-9C7A5A4E9715}"/>
+    <hyperlink ref="F13" r:id="rId9" xr:uid="{3F6BC4D3-5C01-42E1-BAAE-22E95C88ABA7}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{BE3B5412-4D10-4B45-8A97-85CEDE76590E}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{43324E7F-AEB3-458B-9EB2-A7EB91E07129}"/>
+    <hyperlink ref="F16" r:id="rId12" xr:uid="{7E1A8E72-B63B-433C-85DA-77DF0D40C0E9}"/>
+    <hyperlink ref="F18" r:id="rId13" xr:uid="{FE65543E-8C84-42E6-9C5E-5972BEE20845}"/>
+    <hyperlink ref="F19" r:id="rId14" xr:uid="{BBCA4722-2975-4962-A3A7-30DD9E8F81F7}"/>
+    <hyperlink ref="F20" r:id="rId15" xr:uid="{002A2304-1410-42DC-831F-0935A8DEE76E}"/>
+    <hyperlink ref="F21" r:id="rId16" xr:uid="{48C8747D-4EF5-4EC5-8089-C6719FCB9EAB}"/>
+    <hyperlink ref="F22" r:id="rId17" xr:uid="{D700FE5A-99C9-4AA6-AB62-15C9DA75DFE8}"/>
+    <hyperlink ref="F23" r:id="rId18" xr:uid="{083FEA0F-50BD-4852-8492-AEC0CBE51725}"/>
+    <hyperlink ref="F24" r:id="rId19" xr:uid="{23F0E776-957F-4B17-88D7-08E8AB8FEB15}"/>
+    <hyperlink ref="F25" r:id="rId20" xr:uid="{D8322621-6138-48D1-8D3D-FACBE1987851}"/>
+    <hyperlink ref="F26" r:id="rId21" xr:uid="{3FF1CEC4-58DA-41F2-9DAF-C2CB0D4E1143}"/>
+    <hyperlink ref="F27" r:id="rId22" xr:uid="{9D7DAC82-B880-462B-843B-93B8DE4DDAF9}"/>
+    <hyperlink ref="F28" r:id="rId23" xr:uid="{390A535F-1910-49D6-86BD-5B10A562B675}"/>
+    <hyperlink ref="F29" r:id="rId24" xr:uid="{33A7F753-3544-4BF3-BF8B-370F5B2FEA2B}"/>
+    <hyperlink ref="F17" r:id="rId25" xr:uid="{A356E36B-59ED-4429-AD13-B04BE8B514A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84AF481-944A-4A4E-812B-EDDAA2A2EDA1}">
   <dimension ref="G8:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="8" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G8">
         <f>20*2.03</f>
         <v>40.599999999999994</v>
       </c>
     </row>
-    <row r="9" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G9">
         <f>25*1.85</f>
         <v>46.25</v>

</xml_diff>